<commit_message>
using the range names in formulas
</commit_message>
<xml_diff>
--- a/Working with functions and formulas.xlsx
+++ b/Working with functions and formulas.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\Microsoft Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD53FC8-CF3A-44CC-8538-F86D7CD84058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF88EFCC-5BDB-4FA5-902D-94C5F00F6E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{BFDFF372-CC16-4BA7-8A1D-411E9971C80E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="Cost">Sheet1!$J$6:$J$9</definedName>
+    <definedName name="Price">Sheet1!$H$6:$H$9</definedName>
+    <definedName name="Prices">Sheet1!$H$6:$H$9</definedName>
+    <definedName name="Quantity">Sheet1!$I$6:$I$9</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,8 +39,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Pricing Sheet</t>
   </si>
@@ -73,17 +101,28 @@
   </si>
   <si>
     <t>BT306</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity </t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +153,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -123,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -140,12 +187,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -170,9 +227,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -485,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85FF1A5-21D3-412E-B559-005A25CA695E}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,14 +565,15 @@
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -513,7 +581,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="9" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -535,8 +603,18 @@
       <c r="G5" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="H5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -561,8 +639,18 @@
         <f>E6-F6</f>
         <v>45.5715</v>
       </c>
+      <c r="H6" s="11">
+        <v>2.99</v>
+      </c>
+      <c r="I6" s="12">
+        <v>5</v>
+      </c>
+      <c r="J6" s="11" cm="1">
+        <f t="array" ref="J6:J9">Price*Quantity</f>
+        <v>14.950000000000001</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -587,8 +675,17 @@
         <f t="shared" ref="G7:G9" si="2">E7-F7</f>
         <v>105.355</v>
       </c>
+      <c r="H7" s="11">
+        <v>34.99</v>
+      </c>
+      <c r="I7" s="12">
+        <v>65</v>
+      </c>
+      <c r="J7" s="11">
+        <v>2274.35</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -613,8 +710,17 @@
         <f t="shared" si="2"/>
         <v>50.140999999999998</v>
       </c>
+      <c r="H8" s="11">
+        <v>42.5</v>
+      </c>
+      <c r="I8" s="12">
+        <v>45</v>
+      </c>
+      <c r="J8" s="11">
+        <v>1912.5</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -638,6 +744,15 @@
       <c r="G9" s="6">
         <f t="shared" si="2"/>
         <v>94.002499999999984</v>
+      </c>
+      <c r="H9" s="13">
+        <v>56.13</v>
+      </c>
+      <c r="I9" s="12">
+        <v>35</v>
+      </c>
+      <c r="J9" s="14">
+        <v>1964.5500000000002</v>
       </c>
     </row>
   </sheetData>
@@ -647,18 +762,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -879,18 +994,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F74B85D-590E-4423-91BD-D02EAD6E3E4E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4CABC4-751D-4CBE-9B96-57B3DC7790DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F74B85D-590E-4423-91BD-D02EAD6E3E4E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
complete a sales worksheet
</commit_message>
<xml_diff>
--- a/Working with functions and formulas.xlsx
+++ b/Working with functions and formulas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\Microsoft Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF88EFCC-5BDB-4FA5-902D-94C5F00F6E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245DD422-80B8-4852-BA94-9DBD668E261D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{BFDFF372-CC16-4BA7-8A1D-411E9971C80E}"/>
+    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10800" xr2:uid="{BFDFF372-CC16-4BA7-8A1D-411E9971C80E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -762,21 +762,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E1CD5F422E388419BB522F4435A2991" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5c10cafc2c37c7f469fd87ac61c85e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b" xmlns:ns3="16c367a0-1ebe-4645-bffe-e50f3117a967" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64cf9e92a51322bbdec604bdb87428eb" ns2:_="" ns3:_="">
     <xsd:import namespace="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b"/>
@@ -993,24 +978,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F74B85D-590E-4423-91BD-D02EAD6E3E4E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4CABC4-751D-4CBE-9B96-57B3DC7790DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98E70E48-4E55-4E6A-B79D-5EEEAC440E62}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1027,4 +1010,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4CABC4-751D-4CBE-9B96-57B3DC7790DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F74B85D-590E-4423-91BD-D02EAD6E3E4E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
calculate a payment rate of each loan
</commit_message>
<xml_diff>
--- a/Working with functions and formulas.xlsx
+++ b/Working with functions and formulas.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\Microsoft Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245DD422-80B8-4852-BA94-9DBD668E261D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FCD6CA-63B0-4425-918C-1B27B694D21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10800" xr2:uid="{BFDFF372-CC16-4BA7-8A1D-411E9971C80E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{BFDFF372-CC16-4BA7-8A1D-411E9971C80E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sales" sheetId="1" r:id="rId1"/>
+    <sheet name="Calculate Loans" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Cost">Sheet1!$J$6:$J$9</definedName>
-    <definedName name="Price">Sheet1!$H$6:$H$9</definedName>
-    <definedName name="Prices">Sheet1!$H$6:$H$9</definedName>
-    <definedName name="Quantity">Sheet1!$I$6:$I$9</definedName>
+    <definedName name="Cost">Sales!$J$6:$J$9</definedName>
+    <definedName name="Price">Sales!$H$6:$H$9</definedName>
+    <definedName name="Prices">Sales!$H$6:$H$9</definedName>
+    <definedName name="Quantity">Sales!$I$6:$I$9</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="23">
   <si>
     <t>Pricing Sheet</t>
   </si>
@@ -111,18 +112,40 @@
   <si>
     <t>Cost</t>
   </si>
+  <si>
+    <t>Loan Payment Schedule</t>
+  </si>
+  <si>
+    <t>Amount of Loan</t>
+  </si>
+  <si>
+    <t>Length of Loan (in years)</t>
+  </si>
+  <si>
+    <t>Annual Interest Rate</t>
+  </si>
+  <si>
+    <t>Payment Period</t>
+  </si>
+  <si>
+    <t>Amount of Each Payment</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,21 +179,59 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -188,21 +249,39 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -227,19 +306,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -554,26 +692,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85FF1A5-21D3-412E-B559-005A25CA695E}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -581,7 +719,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="9" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="9" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
@@ -603,18 +741,18 @@
       <c r="G5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -639,18 +777,18 @@
         <f>E6-F6</f>
         <v>45.5715</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <v>2.99</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="11">
         <v>5</v>
       </c>
-      <c r="J6" s="11" cm="1">
+      <c r="J6" s="10" cm="1">
         <f t="array" ref="J6:J9">Price*Quantity</f>
         <v>14.950000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -675,17 +813,17 @@
         <f t="shared" ref="G7:G9" si="2">E7-F7</f>
         <v>105.355</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <v>34.99</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>65</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="10">
         <v>2274.35</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -710,17 +848,17 @@
         <f t="shared" si="2"/>
         <v>50.140999999999998</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>42.5</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="11">
         <v>45</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="10">
         <v>1912.5</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -745,13 +883,13 @@
         <f t="shared" si="2"/>
         <v>94.002499999999984</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="12">
         <v>56.13</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="11">
         <v>35</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="13">
         <v>1964.5500000000002</v>
       </c>
     </row>
@@ -761,7 +899,1728 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E26F5B-2E8E-4AB4-97A6-CC83C28FF7BC}">
+  <dimension ref="C1:G94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="29.08984375" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" customWidth="1"/>
+    <col min="7" max="7" width="23.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="C1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C3" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D3" s="17">
+        <v>3</v>
+      </c>
+      <c r="E3" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="40">
+        <f>PMT(E3/12,D3*12,C3)</f>
+        <v>-1504.16352573206</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C4" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D4" s="17">
+        <v>4</v>
+      </c>
+      <c r="E4" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="40">
+        <f t="shared" ref="G4:G67" si="0">PMT(E4/12,D4*12,C4)</f>
+        <v>-1157.135637550979</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C5" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D5" s="17">
+        <v>5</v>
+      </c>
+      <c r="E5" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="40">
+        <f t="shared" si="0"/>
+        <v>-949.29919217133636</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C6" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D6" s="17">
+        <v>6</v>
+      </c>
+      <c r="E6" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="40">
+        <f t="shared" si="0"/>
+        <v>-811.05768738498045</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C7" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D7" s="17">
+        <v>7</v>
+      </c>
+      <c r="E7" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="40">
+        <f t="shared" si="0"/>
+        <v>-712.58390475524959</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C8" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D8" s="17">
+        <v>8</v>
+      </c>
+      <c r="E8" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="40">
+        <f t="shared" si="0"/>
+        <v>-638.96410864421455</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C9" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D9" s="17">
+        <v>9</v>
+      </c>
+      <c r="E9" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="40">
+        <f t="shared" si="0"/>
+        <v>-581.91277943437024</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C10" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D10" s="17">
+        <v>10</v>
+      </c>
+      <c r="E10" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="40">
+        <f t="shared" si="0"/>
+        <v>-536.45850700376195</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C11" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D11" s="17">
+        <v>11</v>
+      </c>
+      <c r="E11" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="40">
+        <f t="shared" si="0"/>
+        <v>-499.43757883365595</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C12" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D12" s="17">
+        <v>12</v>
+      </c>
+      <c r="E12" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="40">
+        <f t="shared" si="0"/>
+        <v>-468.74077420792958</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C13" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D13" s="17">
+        <v>13</v>
+      </c>
+      <c r="E13" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="40">
+        <f t="shared" si="0"/>
+        <v>-442.90779198801283</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C14" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D14" s="17">
+        <v>14</v>
+      </c>
+      <c r="E14" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="40">
+        <f t="shared" si="0"/>
+        <v>-420.8954951703401</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C15" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D15" s="17">
+        <v>15</v>
+      </c>
+      <c r="E15" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="40">
+        <f t="shared" si="0"/>
+        <v>-401.93885772254777</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C16" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D16" s="17">
+        <v>16</v>
+      </c>
+      <c r="E16" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="40">
+        <f t="shared" si="0"/>
+        <v>-385.46405644624065</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C17" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D17" s="17">
+        <v>17</v>
+      </c>
+      <c r="E17" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="40">
+        <f t="shared" si="0"/>
+        <v>-371.03223637963328</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C18" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D18" s="17">
+        <v>18</v>
+      </c>
+      <c r="E18" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="40">
+        <f t="shared" si="0"/>
+        <v>-358.30202113613717</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C19" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D19" s="17">
+        <v>19</v>
+      </c>
+      <c r="E19" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="40">
+        <f t="shared" si="0"/>
+        <v>-347.00386214487384</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C20" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D20" s="17">
+        <v>20</v>
+      </c>
+      <c r="E20" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="40">
+        <f t="shared" si="0"/>
+        <v>-336.92208317256598</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C21" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D21" s="17">
+        <v>21</v>
+      </c>
+      <c r="E21" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="40">
+        <f t="shared" si="0"/>
+        <v>-327.88205502826634</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C22" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D22" s="17">
+        <v>22</v>
+      </c>
+      <c r="E22" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="40">
+        <f t="shared" si="0"/>
+        <v>-319.74086811541878</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C23" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D23" s="17">
+        <v>23</v>
+      </c>
+      <c r="E23" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="40">
+        <f t="shared" si="0"/>
+        <v>-312.38043826456504</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C24" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D24" s="17">
+        <v>24</v>
+      </c>
+      <c r="E24" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="40">
+        <f t="shared" si="0"/>
+        <v>-305.70233613554984</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C25" s="16">
+        <v>50000</v>
+      </c>
+      <c r="D25" s="17">
+        <v>25</v>
+      </c>
+      <c r="E25" s="18">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="40">
+        <f t="shared" si="0"/>
+        <v>-299.62385758563789</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C26" s="19">
+        <v>100000</v>
+      </c>
+      <c r="D26" s="20">
+        <v>3</v>
+      </c>
+      <c r="E26" s="21">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="40">
+        <f t="shared" si="0"/>
+        <v>-3008.3270514641199</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C27" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D27" s="24">
+        <v>4</v>
+      </c>
+      <c r="E27" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="40">
+        <f t="shared" si="0"/>
+        <v>-2314.2712751019581</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C28" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D28" s="24">
+        <v>5</v>
+      </c>
+      <c r="E28" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="40">
+        <f t="shared" si="0"/>
+        <v>-1898.5983843426727</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C29" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D29" s="24">
+        <v>6</v>
+      </c>
+      <c r="E29" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="40">
+        <f t="shared" si="0"/>
+        <v>-1622.1153747699609</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C30" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D30" s="24">
+        <v>7</v>
+      </c>
+      <c r="E30" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F30" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="40">
+        <f t="shared" si="0"/>
+        <v>-1425.1678095104992</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C31" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D31" s="24">
+        <v>8</v>
+      </c>
+      <c r="E31" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="40">
+        <f t="shared" si="0"/>
+        <v>-1277.9282172884291</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C32" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D32" s="24">
+        <v>9</v>
+      </c>
+      <c r="E32" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="40">
+        <f t="shared" si="0"/>
+        <v>-1163.8255588687405</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C33" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D33" s="24">
+        <v>10</v>
+      </c>
+      <c r="E33" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="40">
+        <f t="shared" si="0"/>
+        <v>-1072.9170140075239</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C34" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D34" s="24">
+        <v>11</v>
+      </c>
+      <c r="E34" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" s="40">
+        <f t="shared" si="0"/>
+        <v>-998.8751576673119</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C35" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D35" s="24">
+        <v>12</v>
+      </c>
+      <c r="E35" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="40">
+        <f t="shared" si="0"/>
+        <v>-937.48154841585915</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C36" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D36" s="24">
+        <v>13</v>
+      </c>
+      <c r="E36" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="40">
+        <f t="shared" si="0"/>
+        <v>-885.81558397602566</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C37" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D37" s="24">
+        <v>14</v>
+      </c>
+      <c r="E37" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" s="40">
+        <f t="shared" si="0"/>
+        <v>-841.7909903406802</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C38" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D38" s="24">
+        <v>15</v>
+      </c>
+      <c r="E38" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" s="40">
+        <f t="shared" si="0"/>
+        <v>-803.87771544509553</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C39" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D39" s="24">
+        <v>16</v>
+      </c>
+      <c r="E39" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F39" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" s="40">
+        <f t="shared" si="0"/>
+        <v>-770.92811289248129</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C40" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D40" s="24">
+        <v>17</v>
+      </c>
+      <c r="E40" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F40" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="40">
+        <f t="shared" si="0"/>
+        <v>-742.06447275926655</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C41" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D41" s="24">
+        <v>18</v>
+      </c>
+      <c r="E41" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F41" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" s="40">
+        <f t="shared" si="0"/>
+        <v>-716.60404227227434</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C42" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D42" s="24">
+        <v>19</v>
+      </c>
+      <c r="E42" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F42" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="40">
+        <f t="shared" si="0"/>
+        <v>-694.00772428974767</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C43" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D43" s="24">
+        <v>20</v>
+      </c>
+      <c r="E43" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F43" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" s="40">
+        <f t="shared" si="0"/>
+        <v>-673.84416634513195</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C44" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D44" s="24">
+        <v>21</v>
+      </c>
+      <c r="E44" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F44" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="40">
+        <f t="shared" si="0"/>
+        <v>-655.76411005653267</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C45" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D45" s="24">
+        <v>22</v>
+      </c>
+      <c r="E45" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" s="40">
+        <f t="shared" si="0"/>
+        <v>-639.48173623083756</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C46" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D46" s="24">
+        <v>23</v>
+      </c>
+      <c r="E46" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F46" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" s="40">
+        <f t="shared" si="0"/>
+        <v>-624.76087652913009</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C47" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D47" s="24">
+        <v>24</v>
+      </c>
+      <c r="E47" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" s="40">
+        <f t="shared" si="0"/>
+        <v>-611.40467227109968</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C48" s="23">
+        <v>100000</v>
+      </c>
+      <c r="D48" s="24">
+        <v>25</v>
+      </c>
+      <c r="E48" s="25">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F48" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="40">
+        <f t="shared" si="0"/>
+        <v>-599.24771517127579</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C49" s="26">
+        <v>150000</v>
+      </c>
+      <c r="D49" s="27">
+        <v>3</v>
+      </c>
+      <c r="E49" s="28">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F49" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G49" s="40">
+        <f t="shared" si="0"/>
+        <v>-4512.4905771961803</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C50" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D50" s="31">
+        <v>4</v>
+      </c>
+      <c r="E50" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F50" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50" s="40">
+        <f t="shared" si="0"/>
+        <v>-3471.4069126529366</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C51" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D51" s="31">
+        <v>5</v>
+      </c>
+      <c r="E51" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F51" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G51" s="40">
+        <f t="shared" si="0"/>
+        <v>-2847.8975765140094</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C52" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D52" s="31">
+        <v>6</v>
+      </c>
+      <c r="E52" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F52" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" s="40">
+        <f t="shared" si="0"/>
+        <v>-2433.1730621549414</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C53" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D53" s="31">
+        <v>7</v>
+      </c>
+      <c r="E53" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F53" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="40">
+        <f t="shared" si="0"/>
+        <v>-2137.7517142657489</v>
+      </c>
+    </row>
+    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C54" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D54" s="31">
+        <v>8</v>
+      </c>
+      <c r="E54" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F54" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G54" s="40">
+        <f t="shared" si="0"/>
+        <v>-1916.8923259326434</v>
+      </c>
+    </row>
+    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C55" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D55" s="31">
+        <v>9</v>
+      </c>
+      <c r="E55" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F55" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" s="40">
+        <f t="shared" si="0"/>
+        <v>-1745.738338303111</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C56" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D56" s="31">
+        <v>10</v>
+      </c>
+      <c r="E56" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F56" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56" s="40">
+        <f t="shared" si="0"/>
+        <v>-1609.3755210112856</v>
+      </c>
+    </row>
+    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C57" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D57" s="31">
+        <v>11</v>
+      </c>
+      <c r="E57" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F57" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G57" s="40">
+        <f t="shared" si="0"/>
+        <v>-1498.312736500968</v>
+      </c>
+    </row>
+    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C58" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D58" s="31">
+        <v>12</v>
+      </c>
+      <c r="E58" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F58" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G58" s="40">
+        <f t="shared" si="0"/>
+        <v>-1406.2223226237888</v>
+      </c>
+    </row>
+    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C59" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D59" s="31">
+        <v>13</v>
+      </c>
+      <c r="E59" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F59" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G59" s="40">
+        <f t="shared" si="0"/>
+        <v>-1328.7233759640385</v>
+      </c>
+    </row>
+    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C60" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D60" s="31">
+        <v>14</v>
+      </c>
+      <c r="E60" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F60" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G60" s="40">
+        <f t="shared" si="0"/>
+        <v>-1262.6864855110202</v>
+      </c>
+    </row>
+    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C61" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D61" s="31">
+        <v>15</v>
+      </c>
+      <c r="E61" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F61" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G61" s="40">
+        <f t="shared" si="0"/>
+        <v>-1205.8165731676431</v>
+      </c>
+    </row>
+    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C62" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D62" s="31">
+        <v>16</v>
+      </c>
+      <c r="E62" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F62" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G62" s="40">
+        <f t="shared" si="0"/>
+        <v>-1156.3921693387222</v>
+      </c>
+    </row>
+    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C63" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D63" s="31">
+        <v>17</v>
+      </c>
+      <c r="E63" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F63" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G63" s="40">
+        <f t="shared" si="0"/>
+        <v>-1113.0967091388998</v>
+      </c>
+    </row>
+    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C64" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D64" s="31">
+        <v>18</v>
+      </c>
+      <c r="E64" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F64" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G64" s="40">
+        <f t="shared" si="0"/>
+        <v>-1074.9060634084115</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C65" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D65" s="31">
+        <v>19</v>
+      </c>
+      <c r="E65" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F65" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G65" s="40">
+        <f t="shared" si="0"/>
+        <v>-1041.0115864346214</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C66" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D66" s="31">
+        <v>20</v>
+      </c>
+      <c r="E66" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F66" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G66" s="40">
+        <f t="shared" si="0"/>
+        <v>-1010.766249517698</v>
+      </c>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C67" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D67" s="31">
+        <v>21</v>
+      </c>
+      <c r="E67" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F67" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G67" s="40">
+        <f t="shared" si="0"/>
+        <v>-983.64616508479889</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C68" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D68" s="31">
+        <v>22</v>
+      </c>
+      <c r="E68" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F68" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="40">
+        <f t="shared" ref="G68:G94" si="1">PMT(E68/12,D68*12,C68)</f>
+        <v>-959.22260434625628</v>
+      </c>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C69" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D69" s="31">
+        <v>23</v>
+      </c>
+      <c r="E69" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F69" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G69" s="40">
+        <f t="shared" si="1"/>
+        <v>-937.1413147936953</v>
+      </c>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C70" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D70" s="31">
+        <v>24</v>
+      </c>
+      <c r="E70" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F70" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G70" s="40">
+        <f t="shared" si="1"/>
+        <v>-917.10700840664958</v>
+      </c>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C71" s="30">
+        <v>150000</v>
+      </c>
+      <c r="D71" s="31">
+        <v>25</v>
+      </c>
+      <c r="E71" s="32">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F71" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G71" s="40">
+        <f t="shared" si="1"/>
+        <v>-898.87157275691379</v>
+      </c>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C72" s="33">
+        <v>200000</v>
+      </c>
+      <c r="D72" s="34">
+        <v>3</v>
+      </c>
+      <c r="E72" s="35">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F72" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="G72" s="40">
+        <f t="shared" si="1"/>
+        <v>-6016.6541029282398</v>
+      </c>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C73" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D73" s="38">
+        <v>4</v>
+      </c>
+      <c r="E73" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F73" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G73" s="40">
+        <f t="shared" si="1"/>
+        <v>-4628.5425502039161</v>
+      </c>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C74" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D74" s="38">
+        <v>5</v>
+      </c>
+      <c r="E74" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F74" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G74" s="40">
+        <f t="shared" si="1"/>
+        <v>-3797.1967686853454</v>
+      </c>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C75" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D75" s="38">
+        <v>6</v>
+      </c>
+      <c r="E75" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F75" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G75" s="40">
+        <f t="shared" si="1"/>
+        <v>-3244.2307495399218</v>
+      </c>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C76" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D76" s="38">
+        <v>7</v>
+      </c>
+      <c r="E76" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F76" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G76" s="40">
+        <f t="shared" si="1"/>
+        <v>-2850.3356190209984</v>
+      </c>
+    </row>
+    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C77" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D77" s="38">
+        <v>8</v>
+      </c>
+      <c r="E77" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F77" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G77" s="40">
+        <f t="shared" si="1"/>
+        <v>-2555.8564345768582</v>
+      </c>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C78" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D78" s="38">
+        <v>9</v>
+      </c>
+      <c r="E78" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F78" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G78" s="40">
+        <f t="shared" si="1"/>
+        <v>-2327.6511177374809</v>
+      </c>
+    </row>
+    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C79" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D79" s="38">
+        <v>10</v>
+      </c>
+      <c r="E79" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F79" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G79" s="40">
+        <f t="shared" si="1"/>
+        <v>-2145.8340280150478</v>
+      </c>
+    </row>
+    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C80" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D80" s="38">
+        <v>11</v>
+      </c>
+      <c r="E80" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F80" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G80" s="40">
+        <f t="shared" si="1"/>
+        <v>-1997.7503153346238</v>
+      </c>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C81" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D81" s="38">
+        <v>12</v>
+      </c>
+      <c r="E81" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F81" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G81" s="40">
+        <f t="shared" si="1"/>
+        <v>-1874.9630968317183</v>
+      </c>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C82" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D82" s="38">
+        <v>13</v>
+      </c>
+      <c r="E82" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F82" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G82" s="40">
+        <f t="shared" si="1"/>
+        <v>-1771.6311679520513</v>
+      </c>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C83" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D83" s="38">
+        <v>14</v>
+      </c>
+      <c r="E83" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F83" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G83" s="40">
+        <f t="shared" si="1"/>
+        <v>-1683.5819806813604</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C84" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D84" s="38">
+        <v>15</v>
+      </c>
+      <c r="E84" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F84" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G84" s="40">
+        <f t="shared" si="1"/>
+        <v>-1607.7554308901911</v>
+      </c>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C85" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D85" s="38">
+        <v>16</v>
+      </c>
+      <c r="E85" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F85" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G85" s="40">
+        <f t="shared" si="1"/>
+        <v>-1541.8562257849626</v>
+      </c>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C86" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D86" s="38">
+        <v>17</v>
+      </c>
+      <c r="E86" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F86" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G86" s="40">
+        <f t="shared" si="1"/>
+        <v>-1484.1289455185331</v>
+      </c>
+    </row>
+    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C87" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D87" s="38">
+        <v>18</v>
+      </c>
+      <c r="E87" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F87" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G87" s="40">
+        <f t="shared" si="1"/>
+        <v>-1433.2080845445487</v>
+      </c>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C88" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D88" s="38">
+        <v>19</v>
+      </c>
+      <c r="E88" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F88" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G88" s="40">
+        <f t="shared" si="1"/>
+        <v>-1388.0154485794953</v>
+      </c>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C89" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D89" s="38">
+        <v>20</v>
+      </c>
+      <c r="E89" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F89" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G89" s="40">
+        <f t="shared" si="1"/>
+        <v>-1347.6883326902639</v>
+      </c>
+    </row>
+    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C90" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D90" s="38">
+        <v>21</v>
+      </c>
+      <c r="E90" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F90" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G90" s="40">
+        <f t="shared" si="1"/>
+        <v>-1311.5282201130653</v>
+      </c>
+    </row>
+    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C91" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D91" s="38">
+        <v>22</v>
+      </c>
+      <c r="E91" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F91" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G91" s="40">
+        <f t="shared" si="1"/>
+        <v>-1278.9634724616751</v>
+      </c>
+    </row>
+    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C92" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D92" s="38">
+        <v>23</v>
+      </c>
+      <c r="E92" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F92" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G92" s="40">
+        <f t="shared" si="1"/>
+        <v>-1249.5217530582602</v>
+      </c>
+    </row>
+    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C93" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D93" s="38">
+        <v>24</v>
+      </c>
+      <c r="E93" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F93" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G93" s="40">
+        <f t="shared" si="1"/>
+        <v>-1222.8093445421994</v>
+      </c>
+    </row>
+    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C94" s="37">
+        <v>200000</v>
+      </c>
+      <c r="D94" s="38">
+        <v>25</v>
+      </c>
+      <c r="E94" s="39">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F94" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="G94" s="40">
+        <f t="shared" si="1"/>
+        <v>-1198.4954303425516</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E1CD5F422E388419BB522F4435A2991" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5c10cafc2c37c7f469fd87ac61c85e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b" xmlns:ns3="16c367a0-1ebe-4645-bffe-e50f3117a967" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64cf9e92a51322bbdec604bdb87428eb" ns2:_="" ns3:_="">
     <xsd:import namespace="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b"/>
@@ -978,22 +2837,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F74B85D-590E-4423-91BD-D02EAD6E3E4E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4CABC4-751D-4CBE-9B96-57B3DC7790DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98E70E48-4E55-4E6A-B79D-5EEEAC440E62}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1010,21 +2871,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4CABC4-751D-4CBE-9B96-57B3DC7790DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F74B85D-590E-4423-91BD-D02EAD6E3E4E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
analyzing data using text functions
</commit_message>
<xml_diff>
--- a/Working with functions and formulas.xlsx
+++ b/Working with functions and formulas.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\Microsoft Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FCD6CA-63B0-4425-918C-1B27B694D21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6C90D7-49B5-47C1-9F00-1A3541F1599B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{BFDFF372-CC16-4BA7-8A1D-411E9971C80E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{BFDFF372-CC16-4BA7-8A1D-411E9971C80E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sales" sheetId="1" r:id="rId1"/>
-    <sheet name="Calculate Loans" sheetId="2" r:id="rId2"/>
+    <sheet name="Original Dataset" sheetId="4" r:id="rId1"/>
+    <sheet name="Sales" sheetId="1" r:id="rId2"/>
+    <sheet name="Calculate Loans" sheetId="2" r:id="rId3"/>
+    <sheet name="Automate " sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Cost">Sales!$J$6:$J$9</definedName>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="35">
   <si>
     <t>Pricing Sheet</t>
   </si>
@@ -132,6 +134,42 @@
   </si>
   <si>
     <t>Monthly</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>First Initial</t>
+  </si>
+  <si>
+    <t>Last Initial</t>
+  </si>
+  <si>
+    <t>Full Initals</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Invoice #:</t>
+  </si>
+  <si>
+    <t>Shipment Method:</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Johnson</t>
   </si>
 </sst>
 </file>
@@ -281,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -312,9 +350,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -375,6 +410,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -689,11 +742,1715 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B6B045-7737-490B-BA1C-7A3845F8DD5E}">
+  <dimension ref="A1:J110"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.08984375" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" customWidth="1"/>
+    <col min="7" max="7" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="42">
+        <v>42320</v>
+      </c>
+      <c r="G2" s="11">
+        <v>8463157</v>
+      </c>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="42">
+        <v>42321</v>
+      </c>
+      <c r="G3" s="11">
+        <v>45678</v>
+      </c>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3">
+        <v>12.99</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4">
+        <v>3</v>
+      </c>
+      <c r="E9" s="5">
+        <f>(B9+C9)*D9</f>
+        <v>47.97</v>
+      </c>
+      <c r="F9" s="6">
+        <f>E9*$B$6</f>
+        <v>2.3985000000000003</v>
+      </c>
+      <c r="G9" s="6">
+        <f>E9-F9</f>
+        <v>45.5715</v>
+      </c>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.59</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>10</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" ref="E10:E12" si="0">(B10+C10)*D10</f>
+        <v>110.9</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" ref="F10:F12" si="1">E10*$B$6</f>
+        <v>5.5450000000000008</v>
+      </c>
+      <c r="G10" s="6">
+        <f t="shared" ref="G10:G12" si="2">E10-F10</f>
+        <v>105.355</v>
+      </c>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3">
+        <v>22.89</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="0"/>
+        <v>52.78</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="1"/>
+        <v>2.6390000000000002</v>
+      </c>
+      <c r="G11" s="6">
+        <f t="shared" si="2"/>
+        <v>50.140999999999998</v>
+      </c>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3">
+        <v>16.79</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>98.949999999999989</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="1"/>
+        <v>4.9474999999999998</v>
+      </c>
+      <c r="G12" s="6">
+        <f t="shared" si="2"/>
+        <v>94.002499999999984</v>
+      </c>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="43"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="43"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="43"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="43"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+    </row>
+    <row r="17" spans="3:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="C17" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C19" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D19" s="11">
+        <v>3</v>
+      </c>
+      <c r="E19" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C20" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D20" s="11">
+        <v>4</v>
+      </c>
+      <c r="E20" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C21" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D21" s="11">
+        <v>5</v>
+      </c>
+      <c r="E21" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C22" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D22" s="11">
+        <v>6</v>
+      </c>
+      <c r="E22" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C23" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D23" s="11">
+        <v>7</v>
+      </c>
+      <c r="E23" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C24" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D24" s="11">
+        <v>8</v>
+      </c>
+      <c r="E24" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C25" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D25" s="11">
+        <v>9</v>
+      </c>
+      <c r="E25" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C26" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D26" s="11">
+        <v>10</v>
+      </c>
+      <c r="E26" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C27" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D27" s="11">
+        <v>11</v>
+      </c>
+      <c r="E27" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C28" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D28" s="11">
+        <v>12</v>
+      </c>
+      <c r="E28" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C29" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D29" s="11">
+        <v>13</v>
+      </c>
+      <c r="E29" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C30" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D30" s="11">
+        <v>14</v>
+      </c>
+      <c r="E30" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C31" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D31" s="11">
+        <v>15</v>
+      </c>
+      <c r="E31" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C32" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D32" s="11">
+        <v>16</v>
+      </c>
+      <c r="E32" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C33" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D33" s="11">
+        <v>17</v>
+      </c>
+      <c r="E33" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C34" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D34" s="11">
+        <v>18</v>
+      </c>
+      <c r="E34" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C35" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D35" s="11">
+        <v>19</v>
+      </c>
+      <c r="E35" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C36" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D36" s="11">
+        <v>20</v>
+      </c>
+      <c r="E36" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C37" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D37" s="11">
+        <v>21</v>
+      </c>
+      <c r="E37" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C38" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D38" s="11">
+        <v>22</v>
+      </c>
+      <c r="E38" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C39" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D39" s="11">
+        <v>23</v>
+      </c>
+      <c r="E39" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C40" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D40" s="11">
+        <v>24</v>
+      </c>
+      <c r="E40" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C41" s="11">
+        <v>50000</v>
+      </c>
+      <c r="D41" s="11">
+        <v>25</v>
+      </c>
+      <c r="E41" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C42" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D42" s="11">
+        <v>3</v>
+      </c>
+      <c r="E42" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C43" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D43" s="11">
+        <v>4</v>
+      </c>
+      <c r="E43" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C44" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D44" s="11">
+        <v>5</v>
+      </c>
+      <c r="E44" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C45" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D45" s="11">
+        <v>6</v>
+      </c>
+      <c r="E45" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" s="11"/>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C46" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D46" s="11">
+        <v>7</v>
+      </c>
+      <c r="E46" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" s="11"/>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C47" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D47" s="11">
+        <v>8</v>
+      </c>
+      <c r="E47" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" s="11"/>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C48" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D48" s="11">
+        <v>9</v>
+      </c>
+      <c r="E48" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="11"/>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C49" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D49" s="11">
+        <v>10</v>
+      </c>
+      <c r="E49" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C50" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D50" s="11">
+        <v>11</v>
+      </c>
+      <c r="E50" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50" s="11"/>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C51" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D51" s="11">
+        <v>12</v>
+      </c>
+      <c r="E51" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G51" s="11"/>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C52" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D52" s="11">
+        <v>13</v>
+      </c>
+      <c r="E52" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" s="11"/>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C53" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D53" s="11">
+        <v>14</v>
+      </c>
+      <c r="E53" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="11"/>
+    </row>
+    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C54" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D54" s="11">
+        <v>15</v>
+      </c>
+      <c r="E54" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G54" s="11"/>
+    </row>
+    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C55" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D55" s="11">
+        <v>16</v>
+      </c>
+      <c r="E55" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" s="11"/>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C56" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D56" s="11">
+        <v>17</v>
+      </c>
+      <c r="E56" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56" s="11"/>
+    </row>
+    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C57" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D57" s="11">
+        <v>18</v>
+      </c>
+      <c r="E57" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G57" s="11"/>
+    </row>
+    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C58" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D58" s="11">
+        <v>19</v>
+      </c>
+      <c r="E58" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G58" s="11"/>
+    </row>
+    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C59" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D59" s="11">
+        <v>20</v>
+      </c>
+      <c r="E59" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G59" s="11"/>
+    </row>
+    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C60" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D60" s="11">
+        <v>21</v>
+      </c>
+      <c r="E60" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G60" s="11"/>
+    </row>
+    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C61" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D61" s="11">
+        <v>22</v>
+      </c>
+      <c r="E61" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G61" s="11"/>
+    </row>
+    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C62" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D62" s="11">
+        <v>23</v>
+      </c>
+      <c r="E62" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F62" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G62" s="11"/>
+    </row>
+    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C63" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D63" s="11">
+        <v>24</v>
+      </c>
+      <c r="E63" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G63" s="11"/>
+    </row>
+    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C64" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D64" s="11">
+        <v>25</v>
+      </c>
+      <c r="E64" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G64" s="11"/>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C65" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D65" s="11">
+        <v>3</v>
+      </c>
+      <c r="E65" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G65" s="11"/>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C66" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D66" s="11">
+        <v>4</v>
+      </c>
+      <c r="E66" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F66" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G66" s="11"/>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C67" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D67" s="11">
+        <v>5</v>
+      </c>
+      <c r="E67" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G67" s="11"/>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C68" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D68" s="11">
+        <v>6</v>
+      </c>
+      <c r="E68" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F68" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="11"/>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C69" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D69" s="11">
+        <v>7</v>
+      </c>
+      <c r="E69" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G69" s="11"/>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C70" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D70" s="11">
+        <v>8</v>
+      </c>
+      <c r="E70" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G70" s="11"/>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C71" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D71" s="11">
+        <v>9</v>
+      </c>
+      <c r="E71" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G71" s="11"/>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C72" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D72" s="11">
+        <v>10</v>
+      </c>
+      <c r="E72" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F72" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G72" s="11"/>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C73" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D73" s="11">
+        <v>11</v>
+      </c>
+      <c r="E73" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F73" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G73" s="11"/>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C74" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D74" s="11">
+        <v>12</v>
+      </c>
+      <c r="E74" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G74" s="11"/>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C75" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D75" s="11">
+        <v>13</v>
+      </c>
+      <c r="E75" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G75" s="11"/>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C76" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D76" s="11">
+        <v>14</v>
+      </c>
+      <c r="E76" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F76" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G76" s="11"/>
+    </row>
+    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C77" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D77" s="11">
+        <v>15</v>
+      </c>
+      <c r="E77" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F77" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G77" s="11"/>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C78" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D78" s="11">
+        <v>16</v>
+      </c>
+      <c r="E78" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F78" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G78" s="11"/>
+    </row>
+    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C79" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D79" s="11">
+        <v>17</v>
+      </c>
+      <c r="E79" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F79" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G79" s="11"/>
+    </row>
+    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C80" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D80" s="11">
+        <v>18</v>
+      </c>
+      <c r="E80" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F80" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G80" s="11"/>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C81" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D81" s="11">
+        <v>19</v>
+      </c>
+      <c r="E81" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F81" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G81" s="11"/>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C82" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D82" s="11">
+        <v>20</v>
+      </c>
+      <c r="E82" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F82" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G82" s="11"/>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C83" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D83" s="11">
+        <v>21</v>
+      </c>
+      <c r="E83" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F83" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G83" s="11"/>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C84" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D84" s="11">
+        <v>22</v>
+      </c>
+      <c r="E84" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G84" s="11"/>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C85" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D85" s="11">
+        <v>23</v>
+      </c>
+      <c r="E85" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G85" s="11"/>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C86" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D86" s="11">
+        <v>24</v>
+      </c>
+      <c r="E86" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F86" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G86" s="11"/>
+    </row>
+    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C87" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D87" s="11">
+        <v>25</v>
+      </c>
+      <c r="E87" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F87" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G87" s="11"/>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C88" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D88" s="11">
+        <v>3</v>
+      </c>
+      <c r="E88" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F88" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G88" s="11"/>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C89" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D89" s="11">
+        <v>4</v>
+      </c>
+      <c r="E89" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G89" s="11"/>
+    </row>
+    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C90" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D90" s="11">
+        <v>5</v>
+      </c>
+      <c r="E90" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F90" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G90" s="11"/>
+    </row>
+    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C91" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D91" s="11">
+        <v>6</v>
+      </c>
+      <c r="E91" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F91" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G91" s="11"/>
+    </row>
+    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C92" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D92" s="11">
+        <v>7</v>
+      </c>
+      <c r="E92" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F92" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G92" s="11"/>
+    </row>
+    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C93" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D93" s="11">
+        <v>8</v>
+      </c>
+      <c r="E93" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F93" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G93" s="11"/>
+    </row>
+    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C94" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D94" s="11">
+        <v>9</v>
+      </c>
+      <c r="E94" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F94" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G94" s="11"/>
+    </row>
+    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C95" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D95" s="11">
+        <v>10</v>
+      </c>
+      <c r="E95" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F95" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G95" s="11"/>
+    </row>
+    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C96" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D96" s="11">
+        <v>11</v>
+      </c>
+      <c r="E96" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F96" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G96" s="11"/>
+    </row>
+    <row r="97" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C97" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D97" s="11">
+        <v>12</v>
+      </c>
+      <c r="E97" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F97" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G97" s="11"/>
+    </row>
+    <row r="98" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C98" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D98" s="11">
+        <v>13</v>
+      </c>
+      <c r="E98" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F98" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G98" s="11"/>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C99" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D99" s="11">
+        <v>14</v>
+      </c>
+      <c r="E99" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F99" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G99" s="11"/>
+    </row>
+    <row r="100" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C100" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D100" s="11">
+        <v>15</v>
+      </c>
+      <c r="E100" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F100" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G100" s="11"/>
+    </row>
+    <row r="101" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C101" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D101" s="11">
+        <v>16</v>
+      </c>
+      <c r="E101" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F101" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G101" s="11"/>
+    </row>
+    <row r="102" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C102" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D102" s="11">
+        <v>17</v>
+      </c>
+      <c r="E102" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F102" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G102" s="11"/>
+    </row>
+    <row r="103" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C103" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D103" s="11">
+        <v>18</v>
+      </c>
+      <c r="E103" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F103" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G103" s="11"/>
+    </row>
+    <row r="104" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C104" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D104" s="11">
+        <v>19</v>
+      </c>
+      <c r="E104" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F104" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G104" s="11"/>
+    </row>
+    <row r="105" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C105" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D105" s="11">
+        <v>20</v>
+      </c>
+      <c r="E105" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F105" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G105" s="11"/>
+    </row>
+    <row r="106" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C106" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D106" s="11">
+        <v>21</v>
+      </c>
+      <c r="E106" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F106" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G106" s="11"/>
+    </row>
+    <row r="107" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C107" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D107" s="11">
+        <v>22</v>
+      </c>
+      <c r="E107" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F107" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G107" s="11"/>
+    </row>
+    <row r="108" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C108" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D108" s="11">
+        <v>23</v>
+      </c>
+      <c r="E108" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F108" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G108" s="11"/>
+    </row>
+    <row r="109" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C109" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D109" s="11">
+        <v>24</v>
+      </c>
+      <c r="E109" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F109" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G109" s="11"/>
+    </row>
+    <row r="110" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C110" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D110" s="11">
+        <v>25</v>
+      </c>
+      <c r="E110" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F110" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G110" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C17:F17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85FF1A5-21D3-412E-B559-005A25CA695E}">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -766,16 +2523,16 @@
         <v>3</v>
       </c>
       <c r="E6" s="5">
-        <f>(B6+C6)*D6</f>
-        <v>47.97</v>
+        <f>(B6+C6)*'Original Dataset'!CD46</f>
+        <v>0</v>
       </c>
       <c r="F6" s="6">
         <f>E6*$B$3</f>
-        <v>2.3985000000000003</v>
+        <v>0</v>
       </c>
       <c r="G6" s="6">
         <f>E6-F6</f>
-        <v>45.5715</v>
+        <v>0</v>
       </c>
       <c r="H6" s="10">
         <v>2.99</v>
@@ -899,11 +2656,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E26F5B-2E8E-4AB4-97A6-CC83C28FF7BC}">
   <dimension ref="C1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -917,1682 +2674,1682 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C3" s="16">
+      <c r="C3" s="15">
         <v>50000</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <v>3</v>
       </c>
-      <c r="E3" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="40">
+      <c r="E3" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="39">
         <f>PMT(E3/12,D3*12,C3)</f>
         <v>-1504.16352573206</v>
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C4" s="16">
+      <c r="C4" s="15">
         <v>50000</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <v>4</v>
       </c>
-      <c r="E4" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="40">
+      <c r="E4" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="39">
         <f t="shared" ref="G4:G67" si="0">PMT(E4/12,D4*12,C4)</f>
         <v>-1157.135637550979</v>
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C5" s="16">
+      <c r="C5" s="15">
         <v>50000</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <v>5</v>
       </c>
-      <c r="E5" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="40">
+      <c r="E5" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="39">
         <f t="shared" si="0"/>
         <v>-949.29919217133636</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C6" s="16">
+      <c r="C6" s="15">
         <v>50000</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>6</v>
       </c>
-      <c r="E6" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="40">
+      <c r="E6" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="39">
         <f t="shared" si="0"/>
         <v>-811.05768738498045</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C7" s="16">
+      <c r="C7" s="15">
         <v>50000</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>7</v>
       </c>
-      <c r="E7" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="40">
+      <c r="E7" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="39">
         <f t="shared" si="0"/>
         <v>-712.58390475524959</v>
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C8" s="16">
+      <c r="C8" s="15">
         <v>50000</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>8</v>
       </c>
-      <c r="E8" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="40">
+      <c r="E8" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="39">
         <f t="shared" si="0"/>
         <v>-638.96410864421455</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C9" s="16">
+      <c r="C9" s="15">
         <v>50000</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>9</v>
       </c>
-      <c r="E9" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="40">
+      <c r="E9" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="39">
         <f t="shared" si="0"/>
         <v>-581.91277943437024</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <v>50000</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <v>10</v>
       </c>
-      <c r="E10" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="40">
+      <c r="E10" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="39">
         <f t="shared" si="0"/>
         <v>-536.45850700376195</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>50000</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <v>11</v>
       </c>
-      <c r="E11" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="40">
+      <c r="E11" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="39">
         <f t="shared" si="0"/>
         <v>-499.43757883365595</v>
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C12" s="16">
+      <c r="C12" s="15">
         <v>50000</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <v>12</v>
       </c>
-      <c r="E12" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="40">
+      <c r="E12" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="39">
         <f t="shared" si="0"/>
         <v>-468.74077420792958</v>
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C13" s="16">
+      <c r="C13" s="15">
         <v>50000</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <v>13</v>
       </c>
-      <c r="E13" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="40">
+      <c r="E13" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="39">
         <f t="shared" si="0"/>
         <v>-442.90779198801283</v>
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C14" s="16">
+      <c r="C14" s="15">
         <v>50000</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <v>14</v>
       </c>
-      <c r="E14" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="40">
+      <c r="E14" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="39">
         <f t="shared" si="0"/>
         <v>-420.8954951703401</v>
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C15" s="16">
+      <c r="C15" s="15">
         <v>50000</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="16">
         <v>15</v>
       </c>
-      <c r="E15" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="40">
+      <c r="E15" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="39">
         <f t="shared" si="0"/>
         <v>-401.93885772254777</v>
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C16" s="16">
+      <c r="C16" s="15">
         <v>50000</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <v>16</v>
       </c>
-      <c r="E16" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="40">
+      <c r="E16" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="39">
         <f t="shared" si="0"/>
         <v>-385.46405644624065</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="16">
+      <c r="C17" s="15">
         <v>50000</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="16">
         <v>17</v>
       </c>
-      <c r="E17" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="40">
+      <c r="E17" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="39">
         <f t="shared" si="0"/>
         <v>-371.03223637963328</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C18" s="16">
+      <c r="C18" s="15">
         <v>50000</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="16">
         <v>18</v>
       </c>
-      <c r="E18" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="40">
+      <c r="E18" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="39">
         <f t="shared" si="0"/>
         <v>-358.30202113613717</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C19" s="16">
+      <c r="C19" s="15">
         <v>50000</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="16">
         <v>19</v>
       </c>
-      <c r="E19" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="40">
+      <c r="E19" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="39">
         <f t="shared" si="0"/>
         <v>-347.00386214487384</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C20" s="16">
+      <c r="C20" s="15">
         <v>50000</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <v>20</v>
       </c>
-      <c r="E20" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="40">
+      <c r="E20" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="39">
         <f t="shared" si="0"/>
         <v>-336.92208317256598</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C21" s="16">
+      <c r="C21" s="15">
         <v>50000</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="16">
         <v>21</v>
       </c>
-      <c r="E21" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="40">
+      <c r="E21" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="39">
         <f t="shared" si="0"/>
         <v>-327.88205502826634</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C22" s="16">
+      <c r="C22" s="15">
         <v>50000</v>
       </c>
-      <c r="D22" s="17">
-        <v>22</v>
-      </c>
-      <c r="E22" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="40">
+      <c r="D22" s="16">
+        <v>22</v>
+      </c>
+      <c r="E22" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="39">
         <f t="shared" si="0"/>
         <v>-319.74086811541878</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C23" s="16">
+      <c r="C23" s="15">
         <v>50000</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="16">
         <v>23</v>
       </c>
-      <c r="E23" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="40">
+      <c r="E23" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="39">
         <f t="shared" si="0"/>
         <v>-312.38043826456504</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C24" s="16">
+      <c r="C24" s="15">
         <v>50000</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="16">
         <v>24</v>
       </c>
-      <c r="E24" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="40">
+      <c r="E24" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="39">
         <f t="shared" si="0"/>
         <v>-305.70233613554984</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C25" s="16">
+      <c r="C25" s="15">
         <v>50000</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="16">
         <v>25</v>
       </c>
-      <c r="E25" s="18">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="40">
+      <c r="E25" s="17">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="39">
         <f t="shared" si="0"/>
         <v>-299.62385758563789</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C26" s="19">
+      <c r="C26" s="18">
         <v>100000</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="19">
         <v>3</v>
       </c>
-      <c r="E26" s="21">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="40">
+      <c r="E26" s="20">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="39">
         <f t="shared" si="0"/>
         <v>-3008.3270514641199</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C27" s="23">
+      <c r="C27" s="22">
         <v>100000</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="23">
         <v>4</v>
       </c>
-      <c r="E27" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F27" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="40">
+      <c r="E27" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F27" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="39">
         <f t="shared" si="0"/>
         <v>-2314.2712751019581</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C28" s="23">
+      <c r="C28" s="22">
         <v>100000</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="23">
         <v>5</v>
       </c>
-      <c r="E28" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F28" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" s="40">
+      <c r="E28" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="39">
         <f t="shared" si="0"/>
         <v>-1898.5983843426727</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C29" s="23">
+      <c r="C29" s="22">
         <v>100000</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="23">
         <v>6</v>
       </c>
-      <c r="E29" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F29" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G29" s="40">
+      <c r="E29" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="39">
         <f t="shared" si="0"/>
         <v>-1622.1153747699609</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C30" s="23">
+      <c r="C30" s="22">
         <v>100000</v>
       </c>
-      <c r="D30" s="24">
+      <c r="D30" s="23">
         <v>7</v>
       </c>
-      <c r="E30" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F30" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G30" s="40">
+      <c r="E30" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="39">
         <f t="shared" si="0"/>
         <v>-1425.1678095104992</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C31" s="23">
+      <c r="C31" s="22">
         <v>100000</v>
       </c>
-      <c r="D31" s="24">
+      <c r="D31" s="23">
         <v>8</v>
       </c>
-      <c r="E31" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F31" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G31" s="40">
+      <c r="E31" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="39">
         <f t="shared" si="0"/>
         <v>-1277.9282172884291</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C32" s="23">
+      <c r="C32" s="22">
         <v>100000</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="23">
         <v>9</v>
       </c>
-      <c r="E32" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F32" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G32" s="40">
+      <c r="E32" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="39">
         <f t="shared" si="0"/>
         <v>-1163.8255588687405</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C33" s="23">
+      <c r="C33" s="22">
         <v>100000</v>
       </c>
-      <c r="D33" s="24">
+      <c r="D33" s="23">
         <v>10</v>
       </c>
-      <c r="E33" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F33" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G33" s="40">
+      <c r="E33" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="39">
         <f t="shared" si="0"/>
         <v>-1072.9170140075239</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C34" s="23">
+      <c r="C34" s="22">
         <v>100000</v>
       </c>
-      <c r="D34" s="24">
+      <c r="D34" s="23">
         <v>11</v>
       </c>
-      <c r="E34" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F34" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G34" s="40">
+      <c r="E34" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" s="39">
         <f t="shared" si="0"/>
         <v>-998.8751576673119</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C35" s="23">
+      <c r="C35" s="22">
         <v>100000</v>
       </c>
-      <c r="D35" s="24">
+      <c r="D35" s="23">
         <v>12</v>
       </c>
-      <c r="E35" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F35" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G35" s="40">
+      <c r="E35" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="39">
         <f t="shared" si="0"/>
         <v>-937.48154841585915</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C36" s="23">
+      <c r="C36" s="22">
         <v>100000</v>
       </c>
-      <c r="D36" s="24">
+      <c r="D36" s="23">
         <v>13</v>
       </c>
-      <c r="E36" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G36" s="40">
+      <c r="E36" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G36" s="39">
         <f t="shared" si="0"/>
         <v>-885.81558397602566</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C37" s="23">
+      <c r="C37" s="22">
         <v>100000</v>
       </c>
-      <c r="D37" s="24">
+      <c r="D37" s="23">
         <v>14</v>
       </c>
-      <c r="E37" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F37" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G37" s="40">
+      <c r="E37" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" s="39">
         <f t="shared" si="0"/>
         <v>-841.7909903406802</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C38" s="23">
+      <c r="C38" s="22">
         <v>100000</v>
       </c>
-      <c r="D38" s="24">
+      <c r="D38" s="23">
         <v>15</v>
       </c>
-      <c r="E38" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F38" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G38" s="40">
+      <c r="E38" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" s="39">
         <f t="shared" si="0"/>
         <v>-803.87771544509553</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C39" s="23">
+      <c r="C39" s="22">
         <v>100000</v>
       </c>
-      <c r="D39" s="24">
+      <c r="D39" s="23">
         <v>16</v>
       </c>
-      <c r="E39" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F39" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G39" s="40">
+      <c r="E39" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" s="39">
         <f t="shared" si="0"/>
         <v>-770.92811289248129</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C40" s="23">
+      <c r="C40" s="22">
         <v>100000</v>
       </c>
-      <c r="D40" s="24">
+      <c r="D40" s="23">
         <v>17</v>
       </c>
-      <c r="E40" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F40" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="40">
+      <c r="E40" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" s="39">
         <f t="shared" si="0"/>
         <v>-742.06447275926655</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C41" s="23">
+      <c r="C41" s="22">
         <v>100000</v>
       </c>
-      <c r="D41" s="24">
+      <c r="D41" s="23">
         <v>18</v>
       </c>
-      <c r="E41" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F41" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" s="40">
+      <c r="E41" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" s="39">
         <f t="shared" si="0"/>
         <v>-716.60404227227434</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C42" s="23">
+      <c r="C42" s="22">
         <v>100000</v>
       </c>
-      <c r="D42" s="24">
+      <c r="D42" s="23">
         <v>19</v>
       </c>
-      <c r="E42" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G42" s="40">
+      <c r="E42" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="39">
         <f t="shared" si="0"/>
         <v>-694.00772428974767</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C43" s="23">
+      <c r="C43" s="22">
         <v>100000</v>
       </c>
-      <c r="D43" s="24">
+      <c r="D43" s="23">
         <v>20</v>
       </c>
-      <c r="E43" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F43" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G43" s="40">
+      <c r="E43" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" s="39">
         <f t="shared" si="0"/>
         <v>-673.84416634513195</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C44" s="23">
+      <c r="C44" s="22">
         <v>100000</v>
       </c>
-      <c r="D44" s="24">
+      <c r="D44" s="23">
         <v>21</v>
       </c>
-      <c r="E44" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F44" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G44" s="40">
+      <c r="E44" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="39">
         <f t="shared" si="0"/>
         <v>-655.76411005653267</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C45" s="23">
+      <c r="C45" s="22">
         <v>100000</v>
       </c>
-      <c r="D45" s="24">
-        <v>22</v>
-      </c>
-      <c r="E45" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F45" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G45" s="40">
+      <c r="D45" s="23">
+        <v>22</v>
+      </c>
+      <c r="E45" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F45" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" s="39">
         <f t="shared" si="0"/>
         <v>-639.48173623083756</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C46" s="23">
+      <c r="C46" s="22">
         <v>100000</v>
       </c>
-      <c r="D46" s="24">
+      <c r="D46" s="23">
         <v>23</v>
       </c>
-      <c r="E46" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F46" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G46" s="40">
+      <c r="E46" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F46" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" s="39">
         <f t="shared" si="0"/>
         <v>-624.76087652913009</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C47" s="23">
+      <c r="C47" s="22">
         <v>100000</v>
       </c>
-      <c r="D47" s="24">
+      <c r="D47" s="23">
         <v>24</v>
       </c>
-      <c r="E47" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F47" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G47" s="40">
+      <c r="E47" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F47" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" s="39">
         <f t="shared" si="0"/>
         <v>-611.40467227109968</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C48" s="23">
+      <c r="C48" s="22">
         <v>100000</v>
       </c>
-      <c r="D48" s="24">
+      <c r="D48" s="23">
         <v>25</v>
       </c>
-      <c r="E48" s="25">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F48" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="G48" s="40">
+      <c r="E48" s="24">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="39">
         <f t="shared" si="0"/>
         <v>-599.24771517127579</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C49" s="26">
+      <c r="C49" s="25">
         <v>150000</v>
       </c>
-      <c r="D49" s="27">
+      <c r="D49" s="26">
         <v>3</v>
       </c>
-      <c r="E49" s="28">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F49" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="G49" s="40">
+      <c r="E49" s="27">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F49" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G49" s="39">
         <f t="shared" si="0"/>
         <v>-4512.4905771961803</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C50" s="30">
+      <c r="C50" s="29">
         <v>150000</v>
       </c>
-      <c r="D50" s="31">
+      <c r="D50" s="30">
         <v>4</v>
       </c>
-      <c r="E50" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F50" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G50" s="40">
+      <c r="E50" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F50" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50" s="39">
         <f t="shared" si="0"/>
         <v>-3471.4069126529366</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C51" s="30">
+      <c r="C51" s="29">
         <v>150000</v>
       </c>
-      <c r="D51" s="31">
+      <c r="D51" s="30">
         <v>5</v>
       </c>
-      <c r="E51" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F51" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G51" s="40">
+      <c r="E51" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F51" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G51" s="39">
         <f t="shared" si="0"/>
         <v>-2847.8975765140094</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C52" s="30">
+      <c r="C52" s="29">
         <v>150000</v>
       </c>
-      <c r="D52" s="31">
+      <c r="D52" s="30">
         <v>6</v>
       </c>
-      <c r="E52" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F52" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G52" s="40">
+      <c r="E52" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F52" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" s="39">
         <f t="shared" si="0"/>
         <v>-2433.1730621549414</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C53" s="30">
+      <c r="C53" s="29">
         <v>150000</v>
       </c>
-      <c r="D53" s="31">
+      <c r="D53" s="30">
         <v>7</v>
       </c>
-      <c r="E53" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F53" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G53" s="40">
+      <c r="E53" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F53" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="39">
         <f t="shared" si="0"/>
         <v>-2137.7517142657489</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C54" s="30">
+      <c r="C54" s="29">
         <v>150000</v>
       </c>
-      <c r="D54" s="31">
+      <c r="D54" s="30">
         <v>8</v>
       </c>
-      <c r="E54" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F54" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G54" s="40">
+      <c r="E54" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F54" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G54" s="39">
         <f t="shared" si="0"/>
         <v>-1916.8923259326434</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C55" s="30">
+      <c r="C55" s="29">
         <v>150000</v>
       </c>
-      <c r="D55" s="31">
+      <c r="D55" s="30">
         <v>9</v>
       </c>
-      <c r="E55" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F55" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G55" s="40">
+      <c r="E55" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F55" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G55" s="39">
         <f t="shared" si="0"/>
         <v>-1745.738338303111</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C56" s="30">
+      <c r="C56" s="29">
         <v>150000</v>
       </c>
-      <c r="D56" s="31">
+      <c r="D56" s="30">
         <v>10</v>
       </c>
-      <c r="E56" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F56" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G56" s="40">
+      <c r="E56" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F56" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G56" s="39">
         <f t="shared" si="0"/>
         <v>-1609.3755210112856</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C57" s="30">
+      <c r="C57" s="29">
         <v>150000</v>
       </c>
-      <c r="D57" s="31">
+      <c r="D57" s="30">
         <v>11</v>
       </c>
-      <c r="E57" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F57" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G57" s="40">
+      <c r="E57" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F57" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G57" s="39">
         <f t="shared" si="0"/>
         <v>-1498.312736500968</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C58" s="30">
+      <c r="C58" s="29">
         <v>150000</v>
       </c>
-      <c r="D58" s="31">
+      <c r="D58" s="30">
         <v>12</v>
       </c>
-      <c r="E58" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F58" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G58" s="40">
+      <c r="E58" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F58" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G58" s="39">
         <f t="shared" si="0"/>
         <v>-1406.2223226237888</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C59" s="30">
+      <c r="C59" s="29">
         <v>150000</v>
       </c>
-      <c r="D59" s="31">
+      <c r="D59" s="30">
         <v>13</v>
       </c>
-      <c r="E59" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F59" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G59" s="40">
+      <c r="E59" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F59" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G59" s="39">
         <f t="shared" si="0"/>
         <v>-1328.7233759640385</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C60" s="30">
+      <c r="C60" s="29">
         <v>150000</v>
       </c>
-      <c r="D60" s="31">
+      <c r="D60" s="30">
         <v>14</v>
       </c>
-      <c r="E60" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F60" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G60" s="40">
+      <c r="E60" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F60" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G60" s="39">
         <f t="shared" si="0"/>
         <v>-1262.6864855110202</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C61" s="30">
+      <c r="C61" s="29">
         <v>150000</v>
       </c>
-      <c r="D61" s="31">
+      <c r="D61" s="30">
         <v>15</v>
       </c>
-      <c r="E61" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F61" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G61" s="40">
+      <c r="E61" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F61" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G61" s="39">
         <f t="shared" si="0"/>
         <v>-1205.8165731676431</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C62" s="30">
+      <c r="C62" s="29">
         <v>150000</v>
       </c>
-      <c r="D62" s="31">
+      <c r="D62" s="30">
         <v>16</v>
       </c>
-      <c r="E62" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F62" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G62" s="40">
+      <c r="E62" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F62" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G62" s="39">
         <f t="shared" si="0"/>
         <v>-1156.3921693387222</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C63" s="30">
+      <c r="C63" s="29">
         <v>150000</v>
       </c>
-      <c r="D63" s="31">
+      <c r="D63" s="30">
         <v>17</v>
       </c>
-      <c r="E63" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F63" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G63" s="40">
+      <c r="E63" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F63" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G63" s="39">
         <f t="shared" si="0"/>
         <v>-1113.0967091388998</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C64" s="30">
+      <c r="C64" s="29">
         <v>150000</v>
       </c>
-      <c r="D64" s="31">
+      <c r="D64" s="30">
         <v>18</v>
       </c>
-      <c r="E64" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F64" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G64" s="40">
+      <c r="E64" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F64" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G64" s="39">
         <f t="shared" si="0"/>
         <v>-1074.9060634084115</v>
       </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C65" s="30">
+      <c r="C65" s="29">
         <v>150000</v>
       </c>
-      <c r="D65" s="31">
+      <c r="D65" s="30">
         <v>19</v>
       </c>
-      <c r="E65" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F65" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G65" s="40">
+      <c r="E65" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F65" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G65" s="39">
         <f t="shared" si="0"/>
         <v>-1041.0115864346214</v>
       </c>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C66" s="30">
+      <c r="C66" s="29">
         <v>150000</v>
       </c>
-      <c r="D66" s="31">
+      <c r="D66" s="30">
         <v>20</v>
       </c>
-      <c r="E66" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F66" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G66" s="40">
+      <c r="E66" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F66" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G66" s="39">
         <f t="shared" si="0"/>
         <v>-1010.766249517698</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C67" s="30">
+      <c r="C67" s="29">
         <v>150000</v>
       </c>
-      <c r="D67" s="31">
+      <c r="D67" s="30">
         <v>21</v>
       </c>
-      <c r="E67" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F67" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G67" s="40">
+      <c r="E67" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F67" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G67" s="39">
         <f t="shared" si="0"/>
         <v>-983.64616508479889</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C68" s="30">
+      <c r="C68" s="29">
         <v>150000</v>
       </c>
-      <c r="D68" s="31">
-        <v>22</v>
-      </c>
-      <c r="E68" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F68" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G68" s="40">
+      <c r="D68" s="30">
+        <v>22</v>
+      </c>
+      <c r="E68" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F68" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G68" s="39">
         <f t="shared" ref="G68:G94" si="1">PMT(E68/12,D68*12,C68)</f>
         <v>-959.22260434625628</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C69" s="30">
+      <c r="C69" s="29">
         <v>150000</v>
       </c>
-      <c r="D69" s="31">
+      <c r="D69" s="30">
         <v>23</v>
       </c>
-      <c r="E69" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F69" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G69" s="40">
+      <c r="E69" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F69" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G69" s="39">
         <f t="shared" si="1"/>
         <v>-937.1413147936953</v>
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C70" s="30">
+      <c r="C70" s="29">
         <v>150000</v>
       </c>
-      <c r="D70" s="31">
+      <c r="D70" s="30">
         <v>24</v>
       </c>
-      <c r="E70" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F70" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G70" s="40">
+      <c r="E70" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F70" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G70" s="39">
         <f t="shared" si="1"/>
         <v>-917.10700840664958</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C71" s="30">
+      <c r="C71" s="29">
         <v>150000</v>
       </c>
-      <c r="D71" s="31">
+      <c r="D71" s="30">
         <v>25</v>
       </c>
-      <c r="E71" s="32">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F71" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G71" s="40">
+      <c r="E71" s="31">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F71" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="G71" s="39">
         <f t="shared" si="1"/>
         <v>-898.87157275691379</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C72" s="33">
+      <c r="C72" s="32">
         <v>200000</v>
       </c>
-      <c r="D72" s="34">
+      <c r="D72" s="33">
         <v>3</v>
       </c>
-      <c r="E72" s="35">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F72" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="G72" s="40">
+      <c r="E72" s="34">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F72" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G72" s="39">
         <f t="shared" si="1"/>
         <v>-6016.6541029282398</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C73" s="37">
+      <c r="C73" s="36">
         <v>200000</v>
       </c>
-      <c r="D73" s="38">
+      <c r="D73" s="37">
         <v>4</v>
       </c>
-      <c r="E73" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F73" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G73" s="40">
+      <c r="E73" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F73" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G73" s="39">
         <f t="shared" si="1"/>
         <v>-4628.5425502039161</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C74" s="37">
+      <c r="C74" s="36">
         <v>200000</v>
       </c>
-      <c r="D74" s="38">
+      <c r="D74" s="37">
         <v>5</v>
       </c>
-      <c r="E74" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F74" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G74" s="40">
+      <c r="E74" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F74" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G74" s="39">
         <f t="shared" si="1"/>
         <v>-3797.1967686853454</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C75" s="37">
+      <c r="C75" s="36">
         <v>200000</v>
       </c>
-      <c r="D75" s="38">
+      <c r="D75" s="37">
         <v>6</v>
       </c>
-      <c r="E75" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F75" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G75" s="40">
+      <c r="E75" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F75" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G75" s="39">
         <f t="shared" si="1"/>
         <v>-3244.2307495399218</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C76" s="37">
+      <c r="C76" s="36">
         <v>200000</v>
       </c>
-      <c r="D76" s="38">
+      <c r="D76" s="37">
         <v>7</v>
       </c>
-      <c r="E76" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F76" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G76" s="40">
+      <c r="E76" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F76" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G76" s="39">
         <f t="shared" si="1"/>
         <v>-2850.3356190209984</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C77" s="37">
+      <c r="C77" s="36">
         <v>200000</v>
       </c>
-      <c r="D77" s="38">
+      <c r="D77" s="37">
         <v>8</v>
       </c>
-      <c r="E77" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F77" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G77" s="40">
+      <c r="E77" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F77" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G77" s="39">
         <f t="shared" si="1"/>
         <v>-2555.8564345768582</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C78" s="37">
+      <c r="C78" s="36">
         <v>200000</v>
       </c>
-      <c r="D78" s="38">
+      <c r="D78" s="37">
         <v>9</v>
       </c>
-      <c r="E78" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F78" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G78" s="40">
+      <c r="E78" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F78" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G78" s="39">
         <f t="shared" si="1"/>
         <v>-2327.6511177374809</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C79" s="37">
+      <c r="C79" s="36">
         <v>200000</v>
       </c>
-      <c r="D79" s="38">
+      <c r="D79" s="37">
         <v>10</v>
       </c>
-      <c r="E79" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F79" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G79" s="40">
+      <c r="E79" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F79" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G79" s="39">
         <f t="shared" si="1"/>
         <v>-2145.8340280150478</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C80" s="37">
+      <c r="C80" s="36">
         <v>200000</v>
       </c>
-      <c r="D80" s="38">
+      <c r="D80" s="37">
         <v>11</v>
       </c>
-      <c r="E80" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F80" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G80" s="40">
+      <c r="E80" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F80" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G80" s="39">
         <f t="shared" si="1"/>
         <v>-1997.7503153346238</v>
       </c>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C81" s="37">
+      <c r="C81" s="36">
         <v>200000</v>
       </c>
-      <c r="D81" s="38">
+      <c r="D81" s="37">
         <v>12</v>
       </c>
-      <c r="E81" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F81" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G81" s="40">
+      <c r="E81" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F81" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G81" s="39">
         <f t="shared" si="1"/>
         <v>-1874.9630968317183</v>
       </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C82" s="37">
+      <c r="C82" s="36">
         <v>200000</v>
       </c>
-      <c r="D82" s="38">
+      <c r="D82" s="37">
         <v>13</v>
       </c>
-      <c r="E82" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F82" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G82" s="40">
+      <c r="E82" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F82" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G82" s="39">
         <f t="shared" si="1"/>
         <v>-1771.6311679520513</v>
       </c>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C83" s="37">
+      <c r="C83" s="36">
         <v>200000</v>
       </c>
-      <c r="D83" s="38">
+      <c r="D83" s="37">
         <v>14</v>
       </c>
-      <c r="E83" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F83" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G83" s="40">
+      <c r="E83" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F83" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G83" s="39">
         <f t="shared" si="1"/>
         <v>-1683.5819806813604</v>
       </c>
     </row>
     <row r="84" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C84" s="37">
+      <c r="C84" s="36">
         <v>200000</v>
       </c>
-      <c r="D84" s="38">
+      <c r="D84" s="37">
         <v>15</v>
       </c>
-      <c r="E84" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F84" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G84" s="40">
+      <c r="E84" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F84" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G84" s="39">
         <f t="shared" si="1"/>
         <v>-1607.7554308901911</v>
       </c>
     </row>
     <row r="85" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C85" s="37">
+      <c r="C85" s="36">
         <v>200000</v>
       </c>
-      <c r="D85" s="38">
+      <c r="D85" s="37">
         <v>16</v>
       </c>
-      <c r="E85" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F85" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G85" s="40">
+      <c r="E85" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F85" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G85" s="39">
         <f t="shared" si="1"/>
         <v>-1541.8562257849626</v>
       </c>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C86" s="37">
+      <c r="C86" s="36">
         <v>200000</v>
       </c>
-      <c r="D86" s="38">
+      <c r="D86" s="37">
         <v>17</v>
       </c>
-      <c r="E86" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F86" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G86" s="40">
+      <c r="E86" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F86" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G86" s="39">
         <f t="shared" si="1"/>
         <v>-1484.1289455185331</v>
       </c>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C87" s="37">
+      <c r="C87" s="36">
         <v>200000</v>
       </c>
-      <c r="D87" s="38">
+      <c r="D87" s="37">
         <v>18</v>
       </c>
-      <c r="E87" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F87" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G87" s="40">
+      <c r="E87" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F87" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G87" s="39">
         <f t="shared" si="1"/>
         <v>-1433.2080845445487</v>
       </c>
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C88" s="37">
+      <c r="C88" s="36">
         <v>200000</v>
       </c>
-      <c r="D88" s="38">
+      <c r="D88" s="37">
         <v>19</v>
       </c>
-      <c r="E88" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F88" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G88" s="40">
+      <c r="E88" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F88" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G88" s="39">
         <f t="shared" si="1"/>
         <v>-1388.0154485794953</v>
       </c>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C89" s="37">
+      <c r="C89" s="36">
         <v>200000</v>
       </c>
-      <c r="D89" s="38">
+      <c r="D89" s="37">
         <v>20</v>
       </c>
-      <c r="E89" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F89" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G89" s="40">
+      <c r="E89" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F89" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G89" s="39">
         <f t="shared" si="1"/>
         <v>-1347.6883326902639</v>
       </c>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C90" s="37">
+      <c r="C90" s="36">
         <v>200000</v>
       </c>
-      <c r="D90" s="38">
+      <c r="D90" s="37">
         <v>21</v>
       </c>
-      <c r="E90" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F90" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G90" s="40">
+      <c r="E90" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F90" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G90" s="39">
         <f t="shared" si="1"/>
         <v>-1311.5282201130653</v>
       </c>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C91" s="37">
+      <c r="C91" s="36">
         <v>200000</v>
       </c>
-      <c r="D91" s="38">
-        <v>22</v>
-      </c>
-      <c r="E91" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F91" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G91" s="40">
+      <c r="D91" s="37">
+        <v>22</v>
+      </c>
+      <c r="E91" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F91" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G91" s="39">
         <f t="shared" si="1"/>
         <v>-1278.9634724616751</v>
       </c>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C92" s="37">
+      <c r="C92" s="36">
         <v>200000</v>
       </c>
-      <c r="D92" s="38">
+      <c r="D92" s="37">
         <v>23</v>
       </c>
-      <c r="E92" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F92" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G92" s="40">
+      <c r="E92" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F92" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G92" s="39">
         <f t="shared" si="1"/>
         <v>-1249.5217530582602</v>
       </c>
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C93" s="37">
+      <c r="C93" s="36">
         <v>200000</v>
       </c>
-      <c r="D93" s="38">
+      <c r="D93" s="37">
         <v>24</v>
       </c>
-      <c r="E93" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F93" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G93" s="40">
+      <c r="E93" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F93" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G93" s="39">
         <f t="shared" si="1"/>
         <v>-1222.8093445421994</v>
       </c>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C94" s="37">
+      <c r="C94" s="36">
         <v>200000</v>
       </c>
-      <c r="D94" s="38">
+      <c r="D94" s="37">
         <v>25</v>
       </c>
-      <c r="E94" s="39">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F94" s="38" t="s">
-        <v>22</v>
-      </c>
-      <c r="G94" s="40">
+      <c r="E94" s="38">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F94" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G94" s="39">
         <f t="shared" si="1"/>
         <v>-1198.4954303425516</v>
       </c>
@@ -2605,22 +4362,117 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040804AF-6F6A-4EEF-AEB8-7B047F061143}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.6328125" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" customWidth="1"/>
+    <col min="5" max="6" width="15.90625" customWidth="1"/>
+    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+    <col min="8" max="8" width="19.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="41" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="11" t="str">
+        <f>LEFT(A2)</f>
+        <v>J</v>
+      </c>
+      <c r="D2" s="11" t="str">
+        <f>LEFT(B2)</f>
+        <v>S</v>
+      </c>
+      <c r="E2" s="11" t="str">
+        <f>_xlfn.TEXTJOIN(,TRUE,C2,D2)</f>
+        <v>JS</v>
+      </c>
+      <c r="F2" s="42">
+        <v>42320</v>
+      </c>
+      <c r="G2" s="11">
+        <v>8463157</v>
+      </c>
+      <c r="H2" s="11" t="str">
+        <f>IF(LEN(G2)&gt;5,"Rush","Standard")</f>
+        <v>Rush</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="11" t="str">
+        <f>LEFT(A3)</f>
+        <v>J</v>
+      </c>
+      <c r="D3" s="11" t="str">
+        <f>LEFT(B3)</f>
+        <v>J</v>
+      </c>
+      <c r="E3" s="11" t="str">
+        <f>_xlfn.TEXTJOIN(,TRUE,C3,D3)</f>
+        <v>JJ</v>
+      </c>
+      <c r="F3" s="42">
+        <v>42321</v>
+      </c>
+      <c r="G3" s="11">
+        <v>45678</v>
+      </c>
+      <c r="H3" s="11" t="str">
+        <f>IF(LEN(G3)&gt;5,"Rush","Standard")</f>
+        <v>Standard</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E1CD5F422E388419BB522F4435A2991" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5c10cafc2c37c7f469fd87ac61c85e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b" xmlns:ns3="16c367a0-1ebe-4645-bffe-e50f3117a967" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64cf9e92a51322bbdec604bdb87428eb" ns2:_="" ns3:_="">
     <xsd:import namespace="e126d1a7-de2c-4ae3-80af-dc9ec7d9558b"/>
@@ -2837,24 +4689,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F74B85D-590E-4423-91BD-D02EAD6E3E4E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4CABC4-751D-4CBE-9B96-57B3DC7790DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98E70E48-4E55-4E6A-B79D-5EEEAC440E62}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2871,4 +4721,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4CABC4-751D-4CBE-9B96-57B3DC7790DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F74B85D-590E-4423-91BD-D02EAD6E3E4E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
analyze data using logical functions
</commit_message>
<xml_diff>
--- a/Working with functions and formulas.xlsx
+++ b/Working with functions and formulas.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\Microsoft Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6C90D7-49B5-47C1-9F00-1A3541F1599B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99383F98-2222-4CAE-9BD7-546F4517540D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="3" xr2:uid="{BFDFF372-CC16-4BA7-8A1D-411E9971C80E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="4" xr2:uid="{BFDFF372-CC16-4BA7-8A1D-411E9971C80E}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Dataset" sheetId="4" r:id="rId1"/>
     <sheet name="Sales" sheetId="1" r:id="rId2"/>
     <sheet name="Calculate Loans" sheetId="2" r:id="rId3"/>
-    <sheet name="Automate " sheetId="3" r:id="rId4"/>
+    <sheet name="Text Functions" sheetId="3" r:id="rId4"/>
+    <sheet name="Logical Functions" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Cost">Sales!$J$6:$J$9</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="65">
   <si>
     <t>Pricing Sheet</t>
   </si>
@@ -170,20 +171,111 @@
   </si>
   <si>
     <t>Johnson</t>
+  </si>
+  <si>
+    <t>Weekly Sales &amp; Bonus Payout</t>
+  </si>
+  <si>
+    <t>Weekly Bonus Amount</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Call List Comp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekly Sales </t>
+  </si>
+  <si>
+    <t>Weekly Goal</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>Bonus Amount</t>
+  </si>
+  <si>
+    <t>Jackie</t>
+  </si>
+  <si>
+    <t>Williamson</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Bressan</t>
+  </si>
+  <si>
+    <t>Stanley</t>
+  </si>
+  <si>
+    <t>Prestwick</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Jerry</t>
+  </si>
+  <si>
+    <t>Harrison</t>
+  </si>
+  <si>
+    <t>Leah</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>Robyn</t>
+  </si>
+  <si>
+    <t>Fletcher</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>McCain</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>Devon</t>
+  </si>
+  <si>
+    <t>Lawrence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">George </t>
+  </si>
+  <si>
+    <t>Jackson</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="167" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,8 +322,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,6 +373,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,7 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -419,13 +533,27 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -743,15 +871,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B6B045-7737-490B-BA1C-7A3845F8DD5E}">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:L120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.08984375" customWidth="1"/>
@@ -761,7 +889,7 @@
     <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="45" t="s">
         <v>23</v>
       </c>
@@ -787,7 +915,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>31</v>
       </c>
@@ -805,7 +933,7 @@
       </c>
       <c r="H2" s="11"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>33</v>
       </c>
@@ -823,12 +951,12 @@
       </c>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -836,7 +964,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>2</v>
       </c>
@@ -868,7 +996,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -897,7 +1025,7 @@
       <c r="I9" s="44"/>
       <c r="J9" s="44"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -926,7 +1054,7 @@
       <c r="I10" s="44"/>
       <c r="J10" s="44"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -955,7 +1083,7 @@
       <c r="I11" s="44"/>
       <c r="J11" s="44"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -984,7 +1112,7 @@
       <c r="I12" s="44"/>
       <c r="J12" s="44"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="43"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
@@ -994,225 +1122,289 @@
       <c r="G13" s="44"/>
       <c r="H13" s="44"/>
       <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="43"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="43"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="43"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-    </row>
-    <row r="17" spans="3:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="C17" s="40" t="s">
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="13">
+        <v>16785.14</v>
+      </c>
+      <c r="F16" s="13">
+        <v>15000</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="48"/>
+      <c r="J16" s="13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="13">
+        <v>14687.5</v>
+      </c>
+      <c r="F17" s="13">
+        <v>15000</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="48"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="13">
+        <v>13478.96</v>
+      </c>
+      <c r="F18" s="13">
+        <v>15000</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="48"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="13">
+        <v>21689.47</v>
+      </c>
+      <c r="F19" s="13">
+        <v>15000</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="48"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="13">
+        <v>25478.45</v>
+      </c>
+      <c r="F20" s="13">
+        <v>15000</v>
+      </c>
+      <c r="G20" s="13"/>
+      <c r="H20" s="48"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="13">
+        <v>7600</v>
+      </c>
+      <c r="F21" s="13">
+        <v>10000</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="48"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="13">
+        <v>5689</v>
+      </c>
+      <c r="F22" s="13">
+        <v>10000</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="48"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" s="13">
+        <v>12346.87</v>
+      </c>
+      <c r="F23" s="13">
+        <v>10000</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="48"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="13">
+        <v>11687</v>
+      </c>
+      <c r="F24" s="13">
+        <v>10000</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="48"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="13">
+        <v>9874.4500000000007</v>
+      </c>
+      <c r="F25" s="13">
+        <v>10000</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" s="48"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="43"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+    </row>
+    <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C18" s="14" t="s">
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C28" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D28" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E28" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F28" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G28" s="49" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C19" s="11">
-        <v>50000</v>
-      </c>
-      <c r="D19" s="11">
-        <v>3</v>
-      </c>
-      <c r="E19" s="11">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C20" s="11">
-        <v>50000</v>
-      </c>
-      <c r="D20" s="11">
-        <v>4</v>
-      </c>
-      <c r="E20" s="11">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C21" s="11">
-        <v>50000</v>
-      </c>
-      <c r="D21" s="11">
-        <v>5</v>
-      </c>
-      <c r="E21" s="11">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="11"/>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C22" s="11">
-        <v>50000</v>
-      </c>
-      <c r="D22" s="11">
-        <v>6</v>
-      </c>
-      <c r="E22" s="11">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="11"/>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C23" s="11">
-        <v>50000</v>
-      </c>
-      <c r="D23" s="11">
-        <v>7</v>
-      </c>
-      <c r="E23" s="11">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C24" s="11">
-        <v>50000</v>
-      </c>
-      <c r="D24" s="11">
-        <v>8</v>
-      </c>
-      <c r="E24" s="11">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="11"/>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C25" s="11">
-        <v>50000</v>
-      </c>
-      <c r="D25" s="11">
-        <v>9</v>
-      </c>
-      <c r="E25" s="11">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C26" s="11">
-        <v>50000</v>
-      </c>
-      <c r="D26" s="11">
-        <v>10</v>
-      </c>
-      <c r="E26" s="11">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="11"/>
-    </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C27" s="11">
-        <v>50000</v>
-      </c>
-      <c r="D27" s="11">
-        <v>11</v>
-      </c>
-      <c r="E27" s="11">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="11"/>
-    </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C28" s="11">
-        <v>50000</v>
-      </c>
-      <c r="D28" s="11">
-        <v>12</v>
-      </c>
-      <c r="E28" s="11">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C29" s="11">
         <v>50000</v>
       </c>
       <c r="D29" s="11">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E29" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1222,12 +1414,12 @@
       </c>
       <c r="G29" s="11"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C30" s="11">
         <v>50000</v>
       </c>
       <c r="D30" s="11">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E30" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1237,12 +1429,12 @@
       </c>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C31" s="11">
         <v>50000</v>
       </c>
       <c r="D31" s="11">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E31" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1252,12 +1444,12 @@
       </c>
       <c r="G31" s="11"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C32" s="11">
         <v>50000</v>
       </c>
       <c r="D32" s="11">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E32" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1272,7 +1464,7 @@
         <v>50000</v>
       </c>
       <c r="D33" s="11">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E33" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1287,7 +1479,7 @@
         <v>50000</v>
       </c>
       <c r="D34" s="11">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E34" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1302,7 +1494,7 @@
         <v>50000</v>
       </c>
       <c r="D35" s="11">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E35" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1317,7 +1509,7 @@
         <v>50000</v>
       </c>
       <c r="D36" s="11">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E36" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1332,7 +1524,7 @@
         <v>50000</v>
       </c>
       <c r="D37" s="11">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E37" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1347,7 +1539,7 @@
         <v>50000</v>
       </c>
       <c r="D38" s="11">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E38" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1362,7 +1554,7 @@
         <v>50000</v>
       </c>
       <c r="D39" s="11">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E39" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1377,7 +1569,7 @@
         <v>50000</v>
       </c>
       <c r="D40" s="11">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E40" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1392,7 +1584,7 @@
         <v>50000</v>
       </c>
       <c r="D41" s="11">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E41" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1404,10 +1596,10 @@
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="11">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="D42" s="11">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E42" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1419,10 +1611,10 @@
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="11">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="D43" s="11">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E43" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1434,10 +1626,10 @@
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="11">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="D44" s="11">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E44" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1449,10 +1641,10 @@
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="11">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="D45" s="11">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E45" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1464,10 +1656,10 @@
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="11">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="D46" s="11">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E46" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1479,10 +1671,10 @@
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="11">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="D47" s="11">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E47" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1494,10 +1686,10 @@
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="11">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="D48" s="11">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E48" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1509,10 +1701,10 @@
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" s="11">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="D49" s="11">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E49" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1524,10 +1716,10 @@
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" s="11">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="D50" s="11">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E50" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1539,10 +1731,10 @@
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" s="11">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="D51" s="11">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E51" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1557,7 +1749,7 @@
         <v>100000</v>
       </c>
       <c r="D52" s="11">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E52" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1572,7 +1764,7 @@
         <v>100000</v>
       </c>
       <c r="D53" s="11">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E53" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1587,7 +1779,7 @@
         <v>100000</v>
       </c>
       <c r="D54" s="11">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E54" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1602,7 +1794,7 @@
         <v>100000</v>
       </c>
       <c r="D55" s="11">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E55" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1617,7 +1809,7 @@
         <v>100000</v>
       </c>
       <c r="D56" s="11">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E56" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1632,7 +1824,7 @@
         <v>100000</v>
       </c>
       <c r="D57" s="11">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E57" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1647,7 +1839,7 @@
         <v>100000</v>
       </c>
       <c r="D58" s="11">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E58" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1662,7 +1854,7 @@
         <v>100000</v>
       </c>
       <c r="D59" s="11">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E59" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1677,7 +1869,7 @@
         <v>100000</v>
       </c>
       <c r="D60" s="11">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E60" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1692,7 +1884,7 @@
         <v>100000</v>
       </c>
       <c r="D61" s="11">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E61" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1707,7 +1899,7 @@
         <v>100000</v>
       </c>
       <c r="D62" s="11">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E62" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1722,7 +1914,7 @@
         <v>100000</v>
       </c>
       <c r="D63" s="11">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E63" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1737,7 +1929,7 @@
         <v>100000</v>
       </c>
       <c r="D64" s="11">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E64" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1749,10 +1941,10 @@
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C65" s="11">
-        <v>150000</v>
+        <v>100000</v>
       </c>
       <c r="D65" s="11">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E65" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1764,10 +1956,10 @@
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C66" s="11">
-        <v>150000</v>
+        <v>100000</v>
       </c>
       <c r="D66" s="11">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E66" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1779,10 +1971,10 @@
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C67" s="11">
-        <v>150000</v>
+        <v>100000</v>
       </c>
       <c r="D67" s="11">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E67" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1794,10 +1986,10 @@
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C68" s="11">
-        <v>150000</v>
+        <v>100000</v>
       </c>
       <c r="D68" s="11">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E68" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1809,10 +2001,10 @@
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C69" s="11">
-        <v>150000</v>
+        <v>100000</v>
       </c>
       <c r="D69" s="11">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E69" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1824,10 +2016,10 @@
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C70" s="11">
-        <v>150000</v>
+        <v>100000</v>
       </c>
       <c r="D70" s="11">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E70" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1839,10 +2031,10 @@
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C71" s="11">
-        <v>150000</v>
+        <v>100000</v>
       </c>
       <c r="D71" s="11">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E71" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1854,10 +2046,10 @@
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C72" s="11">
-        <v>150000</v>
+        <v>100000</v>
       </c>
       <c r="D72" s="11">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E72" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1869,10 +2061,10 @@
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C73" s="11">
-        <v>150000</v>
+        <v>100000</v>
       </c>
       <c r="D73" s="11">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E73" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1884,10 +2076,10 @@
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C74" s="11">
-        <v>150000</v>
+        <v>100000</v>
       </c>
       <c r="D74" s="11">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E74" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1902,7 +2094,7 @@
         <v>150000</v>
       </c>
       <c r="D75" s="11">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E75" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1917,7 +2109,7 @@
         <v>150000</v>
       </c>
       <c r="D76" s="11">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E76" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1932,7 +2124,7 @@
         <v>150000</v>
       </c>
       <c r="D77" s="11">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E77" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1947,7 +2139,7 @@
         <v>150000</v>
       </c>
       <c r="D78" s="11">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E78" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1962,7 +2154,7 @@
         <v>150000</v>
       </c>
       <c r="D79" s="11">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E79" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1977,7 +2169,7 @@
         <v>150000</v>
       </c>
       <c r="D80" s="11">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E80" s="11">
         <v>5.2499999999999998E-2</v>
@@ -1992,7 +2184,7 @@
         <v>150000</v>
       </c>
       <c r="D81" s="11">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E81" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2007,7 +2199,7 @@
         <v>150000</v>
       </c>
       <c r="D82" s="11">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E82" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2022,7 +2214,7 @@
         <v>150000</v>
       </c>
       <c r="D83" s="11">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E83" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2037,7 +2229,7 @@
         <v>150000</v>
       </c>
       <c r="D84" s="11">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E84" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2052,7 +2244,7 @@
         <v>150000</v>
       </c>
       <c r="D85" s="11">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E85" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2067,7 +2259,7 @@
         <v>150000</v>
       </c>
       <c r="D86" s="11">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E86" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2082,7 +2274,7 @@
         <v>150000</v>
       </c>
       <c r="D87" s="11">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E87" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2094,10 +2286,10 @@
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C88" s="11">
-        <v>200000</v>
+        <v>150000</v>
       </c>
       <c r="D88" s="11">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E88" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2109,10 +2301,10 @@
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C89" s="11">
-        <v>200000</v>
+        <v>150000</v>
       </c>
       <c r="D89" s="11">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E89" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2124,10 +2316,10 @@
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C90" s="11">
-        <v>200000</v>
+        <v>150000</v>
       </c>
       <c r="D90" s="11">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E90" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2139,10 +2331,10 @@
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C91" s="11">
-        <v>200000</v>
+        <v>150000</v>
       </c>
       <c r="D91" s="11">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E91" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2154,10 +2346,10 @@
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C92" s="11">
-        <v>200000</v>
+        <v>150000</v>
       </c>
       <c r="D92" s="11">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E92" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2169,10 +2361,10 @@
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C93" s="11">
-        <v>200000</v>
+        <v>150000</v>
       </c>
       <c r="D93" s="11">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E93" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2184,10 +2376,10 @@
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C94" s="11">
-        <v>200000</v>
+        <v>150000</v>
       </c>
       <c r="D94" s="11">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E94" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2199,10 +2391,10 @@
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C95" s="11">
-        <v>200000</v>
+        <v>150000</v>
       </c>
       <c r="D95" s="11">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E95" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2214,10 +2406,10 @@
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C96" s="11">
-        <v>200000</v>
+        <v>150000</v>
       </c>
       <c r="D96" s="11">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E96" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2229,10 +2421,10 @@
     </row>
     <row r="97" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C97" s="11">
-        <v>200000</v>
+        <v>150000</v>
       </c>
       <c r="D97" s="11">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E97" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2247,7 +2439,7 @@
         <v>200000</v>
       </c>
       <c r="D98" s="11">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E98" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2262,7 +2454,7 @@
         <v>200000</v>
       </c>
       <c r="D99" s="11">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E99" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2277,7 +2469,7 @@
         <v>200000</v>
       </c>
       <c r="D100" s="11">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E100" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2292,7 +2484,7 @@
         <v>200000</v>
       </c>
       <c r="D101" s="11">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="E101" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2307,7 +2499,7 @@
         <v>200000</v>
       </c>
       <c r="D102" s="11">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E102" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2322,7 +2514,7 @@
         <v>200000</v>
       </c>
       <c r="D103" s="11">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E103" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2337,7 +2529,7 @@
         <v>200000</v>
       </c>
       <c r="D104" s="11">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E104" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2352,7 +2544,7 @@
         <v>200000</v>
       </c>
       <c r="D105" s="11">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E105" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2367,7 +2559,7 @@
         <v>200000</v>
       </c>
       <c r="D106" s="11">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E106" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2382,7 +2574,7 @@
         <v>200000</v>
       </c>
       <c r="D107" s="11">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E107" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2397,7 +2589,7 @@
         <v>200000</v>
       </c>
       <c r="D108" s="11">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E108" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2412,7 +2604,7 @@
         <v>200000</v>
       </c>
       <c r="D109" s="11">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E109" s="11">
         <v>5.2499999999999998E-2</v>
@@ -2427,20 +2619,167 @@
         <v>200000</v>
       </c>
       <c r="D110" s="11">
+        <v>15</v>
+      </c>
+      <c r="E110" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F110" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G110" s="11"/>
+    </row>
+    <row r="111" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C111" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D111" s="11">
+        <v>16</v>
+      </c>
+      <c r="E111" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F111" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G111" s="11"/>
+    </row>
+    <row r="112" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C112" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D112" s="11">
+        <v>17</v>
+      </c>
+      <c r="E112" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F112" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G112" s="11"/>
+    </row>
+    <row r="113" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C113" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D113" s="11">
+        <v>18</v>
+      </c>
+      <c r="E113" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F113" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G113" s="11"/>
+    </row>
+    <row r="114" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C114" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D114" s="11">
+        <v>19</v>
+      </c>
+      <c r="E114" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F114" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G114" s="11"/>
+    </row>
+    <row r="115" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C115" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D115" s="11">
+        <v>20</v>
+      </c>
+      <c r="E115" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F115" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G115" s="11"/>
+    </row>
+    <row r="116" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C116" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D116" s="11">
+        <v>21</v>
+      </c>
+      <c r="E116" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F116" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G116" s="11"/>
+    </row>
+    <row r="117" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C117" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D117" s="11">
+        <v>22</v>
+      </c>
+      <c r="E117" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F117" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G117" s="11"/>
+    </row>
+    <row r="118" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C118" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D118" s="11">
+        <v>23</v>
+      </c>
+      <c r="E118" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F118" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G118" s="11"/>
+    </row>
+    <row r="119" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C119" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D119" s="11">
+        <v>24</v>
+      </c>
+      <c r="E119" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F119" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G119" s="11"/>
+    </row>
+    <row r="120" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C120" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D120" s="11">
         <v>25</v>
       </c>
-      <c r="E110" s="11">
-        <v>5.2499999999999998E-2</v>
-      </c>
-      <c r="F110" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G110" s="11"/>
+      <c r="E120" s="11">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="F120" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G120" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C17:F17"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2523,7 +2862,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="5">
-        <f>(B6+C6)*'Original Dataset'!CD46</f>
+        <f>(B6+C6)*'Original Dataset'!CD56</f>
         <v>0</v>
       </c>
       <c r="F6" s="6">
@@ -2674,12 +3013,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
     </row>
     <row r="2" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C2" s="14" t="s">
@@ -4366,8 +4705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{040804AF-6F6A-4EEF-AEB8-7B047F061143}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4468,6 +4807,367 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E697E8CC-73B0-4D04-B4A1-9ECB75041AF2}">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.6328125" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.6">
+      <c r="A1" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="K1" s="47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D2" s="11"/>
+      <c r="K2" s="13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="D3" s="11"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,A5,B5)</f>
+        <v>Jackie_Williamson</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="13">
+        <v>16785.14</v>
+      </c>
+      <c r="F5" s="13">
+        <v>15000</v>
+      </c>
+      <c r="G5" s="13" t="b">
+        <f>AND(D5="Yes",E5&gt;F5)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="48" cm="1">
+        <f t="array" ref="H5:H14">IF(G5:G14=TRUE,K2, 0)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" ref="C6:C14" si="0">_xlfn.TEXTJOIN("_",TRUE,A6,B6)</f>
+        <v>Lucas_Bressan</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="13">
+        <v>14687.5</v>
+      </c>
+      <c r="F6" s="13">
+        <v>15000</v>
+      </c>
+      <c r="G6" s="13" t="b">
+        <f t="shared" ref="G6:G14" si="1">AND(D6="Yes",E6&gt;F6)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>Stanley_Prestwick</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="13">
+        <v>13478.96</v>
+      </c>
+      <c r="F7" s="13">
+        <v>15000</v>
+      </c>
+      <c r="G7" s="13" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>Jerry_Harrison</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="13">
+        <v>21689.47</v>
+      </c>
+      <c r="F8" s="13">
+        <v>15000</v>
+      </c>
+      <c r="G8" s="13" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>Leah_Thompson</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="13">
+        <v>25478.45</v>
+      </c>
+      <c r="F9" s="13">
+        <v>15000</v>
+      </c>
+      <c r="G9" s="13" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="48">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>Robyn_Fletcher</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="13">
+        <v>7600</v>
+      </c>
+      <c r="F10" s="13">
+        <v>10000</v>
+      </c>
+      <c r="G10" s="13" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>Lisa_McCain</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="13">
+        <v>5689</v>
+      </c>
+      <c r="F11" s="13">
+        <v>10000</v>
+      </c>
+      <c r="G11" s="13" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>Steven_Stone</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="13">
+        <v>12346.87</v>
+      </c>
+      <c r="F12" s="13">
+        <v>10000</v>
+      </c>
+      <c r="G12" s="13" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H12" s="48">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>Devon_Lawrence</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="13">
+        <v>11687</v>
+      </c>
+      <c r="F13" s="13">
+        <v>10000</v>
+      </c>
+      <c r="G13" s="13" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>George _Jackson</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="13">
+        <v>9874.4500000000007</v>
+      </c>
+      <c r="F14" s="13">
+        <v>10000</v>
+      </c>
+      <c r="G14" s="13" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="48">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4690,18 +5390,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4724,18 +5424,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F74B85D-590E-4423-91BD-D02EAD6E3E4E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D4CABC4-751D-4CBE-9B96-57B3DC7790DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F74B85D-590E-4423-91BD-D02EAD6E3E4E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>